<commit_message>
updating SUP figures to show percentage and give more meaningful labels
</commit_message>
<xml_diff>
--- a/Papers/LDQ'15 - What's up LOD Cloud - Observing The State of Linked Open Data Cloud Metadata/figures/results_analysis.xlsx
+++ b/Papers/LDQ'15 - What's up LOD Cloud - Observing The State of Linked Open Data Cloud Metadata/figures/results_analysis.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25703"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadassaf/Google Drive/PhD TelecomParisTech - EURECOM - France 2012-2015/My PhD Documents/Papers/LDQ'15 - What's up LOD Cloud - Observing The State of Linked Open Data Cloud Metadata/figures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="19240" yWindow="460" windowWidth="19160" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -211,7 +216,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -260,39 +272,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="23" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -316,6 +331,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="23" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -387,7 +403,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$15:$E$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.3</c:v>
@@ -395,7 +411,7 @@
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0.00">
+                <c:pt idx="2">
                   <c:v>0.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
@@ -444,7 +460,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$16:$E$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.25</c:v>
@@ -498,7 +514,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$17:$E$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.411764705882353</c:v>
@@ -546,7 +562,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$18:$E$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.166666666666667</c:v>
@@ -567,20 +583,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2107258632"/>
-        <c:axId val="2109677176"/>
+        <c:axId val="-2103016208"/>
+        <c:axId val="-2090200320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2107258632"/>
+        <c:axId val="-2103016208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109677176"/>
+        <c:crossAx val="-2090200320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -588,7 +605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109677176"/>
+        <c:axId val="-2090200320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -628,11 +645,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107258632"/>
+        <c:crossAx val="-2103016208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -714,7 +731,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$21:$E$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.3</c:v>
@@ -771,7 +788,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$22:$E$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
@@ -822,7 +839,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$23:$E$23</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.17</c:v>
@@ -870,7 +887,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$24:$E$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.642857142857143</c:v>
@@ -894,20 +911,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2107311064"/>
-        <c:axId val="2107314184"/>
+        <c:axId val="-2090631648"/>
+        <c:axId val="-2090626176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2107311064"/>
+        <c:axId val="-2090631648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107314184"/>
+        <c:crossAx val="-2090626176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -915,7 +933,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107314184"/>
+        <c:axId val="-2090626176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -942,11 +960,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107311064"/>
+        <c:crossAx val="-2090631648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1110,11 +1128,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2107343992"/>
-        <c:axId val="2107349448"/>
+        <c:axId val="-2090245904"/>
+        <c:axId val="-2090503696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2107343992"/>
+        <c:axId val="-2090245904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1139,10 +1157,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107349448"/>
+        <c:crossAx val="-2090503696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1150,7 +1169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107349448"/>
+        <c:axId val="-2090503696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1189,7 +1208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107343992"/>
+        <c:crossAx val="-2090245904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1455,20 +1474,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2124129352"/>
-        <c:axId val="2124130760"/>
+        <c:axId val="-2135881360"/>
+        <c:axId val="-2102109424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2124129352"/>
+        <c:axId val="-2135881360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124130760"/>
+        <c:crossAx val="-2102109424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1476,7 +1496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124130760"/>
+        <c:axId val="-2102109424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124129352"/>
+        <c:crossAx val="-2135881360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1988,11 +2008,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G14" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -2001,7 +2021,7 @@
     <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -2015,7 +2035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2052,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2046,7 +2066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2054,7 +2074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2068,7 +2088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -2096,7 +2116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -2119,7 +2139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2137,7 +2157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -2151,7 +2171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -2167,17 +2187,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="O14" s="1" t="s">
@@ -2193,22 +2214,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <f>3/10</f>
         <v>0.3</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>1</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="5">
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <f>9/14</f>
         <v>0.6428571428571429</v>
       </c>
@@ -2216,45 +2237,51 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>1</v>
       </c>
-      <c r="E16">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5">
         <v>1</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <f>7/17</f>
         <v>0.41176470588235292</v>
       </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
       <c r="N17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E18">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5">
         <f>4/5</f>
         <v>0.8</v>
       </c>
@@ -2262,7 +2289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -2288,23 +2315,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <f>3/10</f>
         <v>0.3</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="5">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="5">
         <f>7/17</f>
         <v>0.41176470588235292</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
@@ -2312,43 +2339,49 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>1</v>
       </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
       <c r="N22" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>0.17</v>
       </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
       <c r="N23" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <f>9/14</f>
         <v>0.6428571428571429</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="5">
         <v>1</v>
       </c>
-      <c r="E24">
+      <c r="D24" s="5"/>
+      <c r="E24" s="5">
         <f>4/5</f>
         <v>0.8</v>
       </c>
@@ -2356,7 +2389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -2364,7 +2397,7 @@
         <v>96.91</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -2393,7 +2426,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -2424,7 +2457,7 @@
         <v>60.300000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -2453,7 +2486,7 @@
         <v>50.018000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2482,7 +2515,7 @@
         <v>53.751999999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -2511,7 +2544,7 @@
         <v>51.204000000000008</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2529,7 +2562,7 @@
         <v>47.96</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -2547,7 +2580,7 @@
         <v>33.729999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -2567,7 +2600,7 @@
         <v>88.01</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -2585,7 +2618,7 @@
         <v>57.12</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -2603,7 +2636,7 @@
         <v>81.97</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>27</v>
       </c>
@@ -2621,7 +2654,7 @@
         <v>7.87</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -2639,7 +2672,7 @@
         <v>15.12</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -2659,7 +2692,7 @@
         <v>88.01</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -2677,7 +2710,7 @@
         <v>57.05</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="J50" s="4"/>
       <c r="K50" t="s">
         <v>49</v>
@@ -2689,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="J51" s="4"/>
       <c r="K51" t="s">
         <v>50</v>
@@ -2701,7 +2734,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="J52" s="4"/>
       <c r="K52" t="s">
         <v>51</v>
@@ -2713,7 +2746,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -2733,7 +2766,7 @@
         <v>79.92</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>32</v>
       </c>
@@ -2751,7 +2784,7 @@
         <v>46.82</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>33</v>
       </c>
@@ -2769,7 +2802,7 @@
         <v>89.29</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -2787,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -2805,7 +2838,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -2823,10 +2856,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding dedicated background chapter for each part and fixing the charts display
</commit_message>
<xml_diff>
--- a/Papers/LDQ'15 - What's up LOD Cloud - Observing The State of Linked Open Data Cloud Metadata/figures/results_analysis.xlsx
+++ b/Papers/LDQ'15 - What's up LOD Cloud - Observing The State of Linked Open Data Cloud Metadata/figures/results_analysis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25703"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -302,10 +302,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="23" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="23" applyFont="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -346,14 +346,14 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -378,7 +378,74 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$14:$E$14</c:f>
@@ -435,7 +502,74 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$14:$E$14</c:f>
@@ -489,7 +623,74 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$14:$E$14</c:f>
@@ -537,7 +738,74 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$14:$E$14</c:f>
@@ -575,29 +843,78 @@
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2103016208"/>
-        <c:axId val="-2090200320"/>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="-2102006640"/>
+        <c:axId val="-2102009920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2103016208"/>
+        <c:axId val="-2102006640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090200320"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2102009920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -605,64 +922,155 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090200320"/>
+        <c:axId val="-2102009920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Metadata</a:t>
+                  <a:t>Metadata fields errors %</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> fields e</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>rrors</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> %</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103016208"/>
+        <c:crossAx val="-2102006640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.527000608293062"/>
+          <c:y val="0.0"/>
+          <c:w val="0.452436551654219"/>
+          <c:h val="0.0743114886229772"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -674,14 +1082,14 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -706,7 +1114,74 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$20:$E$20</c:f>
@@ -763,7 +1238,74 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$20:$E$20</c:f>
@@ -814,7 +1356,74 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$20:$E$20</c:f>
@@ -862,7 +1471,74 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$20:$E$20</c:f>
@@ -903,29 +1579,78 @@
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2090631648"/>
-        <c:axId val="-2090626176"/>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="-2098751824"/>
+        <c:axId val="-2098748640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2090631648"/>
+        <c:axId val="-2098751824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090626176"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2098748640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -933,22 +1658,31 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090626176"/>
+        <c:axId val="-2098748640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
@@ -959,25 +1693,120 @@
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090631648"/>
+        <c:crossAx val="-2098751824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.619714526424937"/>
+          <c:y val="0.0276679841897233"/>
+          <c:w val="0.365509218755063"/>
+          <c:h val="0.0746052099218823"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -989,7 +1818,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1128,11 +1957,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2090245904"/>
-        <c:axId val="-2090503696"/>
+        <c:axId val="-2099512224"/>
+        <c:axId val="-2099507040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2090245904"/>
+        <c:axId val="-2099512224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,7 +1990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090503696"/>
+        <c:crossAx val="-2099507040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1169,7 +1998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090503696"/>
+        <c:axId val="-2099507040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1208,7 +2037,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090245904"/>
+        <c:crossAx val="-2099512224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1228,7 +2057,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1333,7 +2162,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1474,11 +2303,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2135881360"/>
-        <c:axId val="-2102109424"/>
+        <c:axId val="-2099442384"/>
+        <c:axId val="-2099439456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2135881360"/>
+        <c:axId val="-2099442384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1488,7 +2317,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102109424"/>
+        <c:crossAx val="-2099439456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1496,7 +2325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2102109424"/>
+        <c:axId val="-2099439456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1507,7 +2336,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135881360"/>
+        <c:crossAx val="-2099442384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1529,20 +2358,1148 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1569,10 +3526,10 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2008,8 +3965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2188,17 +4145,17 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="O14" s="1" t="s">
@@ -2215,21 +4172,21 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="3">
         <f>3/10</f>
         <v>0.3</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="3">
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="3">
         <f>9/14</f>
         <v>0.6428571428571429</v>
       </c>
@@ -2238,18 +4195,18 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="3">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3">
         <v>1</v>
       </c>
       <c r="N16" s="1" t="s">
@@ -2257,31 +4214,31 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="3">
         <f>7/17</f>
         <v>0.41176470588235292</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
       <c r="N17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="3">
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3">
         <f>4/5</f>
         <v>0.8</v>
       </c>
@@ -2319,19 +4276,19 @@
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="3">
         <f>3/10</f>
         <v>0.3</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="3">
         <f>7/17</f>
         <v>0.41176470588235292</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="3">
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
@@ -2343,14 +4300,14 @@
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="3">
         <v>1</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="3">
         <v>1</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
       <c r="N22" s="1" t="s">
         <v>15</v>
       </c>
@@ -2359,12 +4316,12 @@
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="3">
         <v>0.17</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
       <c r="N23" s="1" t="s">
         <v>14</v>
       </c>
@@ -2373,15 +4330,15 @@
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="3">
         <f>9/14</f>
         <v>0.6428571428571429</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>1</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3">
         <f>4/5</f>
         <v>0.8</v>
       </c>
@@ -2433,7 +4390,7 @@
       <c r="B37" s="2">
         <v>81.55</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="J37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K37" t="s">
@@ -2464,7 +4421,7 @@
       <c r="B38" s="2">
         <v>95.51</v>
       </c>
-      <c r="J38" s="3"/>
+      <c r="J38" s="5"/>
       <c r="K38" t="s">
         <v>37</v>
       </c>
@@ -2493,7 +4450,7 @@
       <c r="B39" s="2">
         <v>6.46</v>
       </c>
-      <c r="J39" s="3"/>
+      <c r="J39" s="5"/>
       <c r="K39" t="s">
         <v>38</v>
       </c>
@@ -2522,7 +4479,7 @@
       <c r="B40" s="2">
         <v>95.88</v>
       </c>
-      <c r="J40" s="3"/>
+      <c r="J40" s="5"/>
       <c r="K40" t="s">
         <v>39</v>
       </c>
@@ -2551,7 +4508,7 @@
       <c r="B41" s="2">
         <v>77.900000000000006</v>
       </c>
-      <c r="J41" s="3"/>
+      <c r="J41" s="5"/>
       <c r="K41" t="s">
         <v>40</v>
       </c>
@@ -2569,7 +4526,7 @@
       <c r="B42" s="2">
         <v>96.91</v>
       </c>
-      <c r="J42" s="3"/>
+      <c r="J42" s="5"/>
       <c r="K42" t="s">
         <v>41</v>
       </c>
@@ -2587,7 +4544,7 @@
       <c r="B43" s="2">
         <v>76.5</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="J43" s="6" t="s">
         <v>10</v>
       </c>
       <c r="K43" t="s">
@@ -2607,7 +4564,7 @@
       <c r="B44" s="2">
         <v>91.29</v>
       </c>
-      <c r="J44" s="4"/>
+      <c r="J44" s="6"/>
       <c r="K44" t="s">
         <v>44</v>
       </c>
@@ -2625,7 +4582,7 @@
       <c r="B45" s="2">
         <v>79.87</v>
       </c>
-      <c r="J45" s="4"/>
+      <c r="J45" s="6"/>
       <c r="K45" t="s">
         <v>45</v>
       </c>
@@ -2643,7 +4600,7 @@
       <c r="B46" s="2">
         <v>45.69</v>
       </c>
-      <c r="J46" s="4"/>
+      <c r="J46" s="6"/>
       <c r="K46" t="s">
         <v>46</v>
       </c>
@@ -2661,7 +4618,7 @@
       <c r="B47" s="2">
         <v>9.18</v>
       </c>
-      <c r="J47" s="4"/>
+      <c r="J47" s="6"/>
       <c r="K47" t="s">
         <v>47</v>
       </c>
@@ -2679,7 +4636,7 @@
       <c r="B48" s="2">
         <v>96.82</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="J48" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K48" t="s">
@@ -2699,7 +4656,7 @@
       <c r="B49" s="2">
         <v>86.8</v>
       </c>
-      <c r="J49" s="4"/>
+      <c r="J49" s="6"/>
       <c r="K49" t="s">
         <v>17</v>
       </c>
@@ -2711,7 +4668,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J50" s="4"/>
+      <c r="J50" s="6"/>
       <c r="K50" t="s">
         <v>49</v>
       </c>
@@ -2723,7 +4680,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J51" s="4"/>
+      <c r="J51" s="6"/>
       <c r="K51" t="s">
         <v>50</v>
       </c>
@@ -2735,7 +4692,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J52" s="4"/>
+      <c r="J52" s="6"/>
       <c r="K52" t="s">
         <v>51</v>
       </c>
@@ -2753,7 +4710,7 @@
       <c r="B53">
         <v>212</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="J53" s="6" t="s">
         <v>8</v>
       </c>
       <c r="K53" t="s">
@@ -2773,7 +4730,7 @@
       <c r="B54">
         <v>8</v>
       </c>
-      <c r="J54" s="4"/>
+      <c r="J54" s="6"/>
       <c r="K54" t="s">
         <v>53</v>
       </c>
@@ -2791,7 +4748,7 @@
       <c r="B55">
         <v>112</v>
       </c>
-      <c r="J55" s="4"/>
+      <c r="J55" s="6"/>
       <c r="K55" t="s">
         <v>54</v>
       </c>
@@ -2809,7 +4766,7 @@
       <c r="B56">
         <v>1</v>
       </c>
-      <c r="J56" s="4"/>
+      <c r="J56" s="6"/>
       <c r="K56" t="s">
         <v>55</v>
       </c>
@@ -2827,7 +4784,7 @@
       <c r="B57">
         <v>1</v>
       </c>
-      <c r="J57" s="4"/>
+      <c r="J57" s="6"/>
       <c r="K57" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
various edits and adding PhD defence presentation
</commit_message>
<xml_diff>
--- a/Papers/LDQ'15 - What's up LOD Cloud - Observing The State of Linked Open Data Cloud Metadata/figures/results_analysis.xlsx
+++ b/Papers/LDQ'15 - What's up LOD Cloud - Observing The State of Linked Open Data Cloud Metadata/figures/results_analysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadassaf/Google Drive/PhD TelecomParisTech - EURECOM - France 2012-2015/My PhD Documents/Papers/LDQ'15 - What's up LOD Cloud - Observing The State of Linked Open Data Cloud Metadata/figures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadassaf/Google Drive/Documents/PhD TelecomParisTech - EURECOM - France 2012-2015/My PhD Documents/Papers/LDQ'15 - What's up LOD Cloud - Observing The State of Linked Open Data Cloud Metadata/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19240" yWindow="460" windowWidth="19160" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -853,11 +853,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="-2102006640"/>
-        <c:axId val="-2102009920"/>
+        <c:axId val="-2058765056"/>
+        <c:axId val="-2132201952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2102006640"/>
+        <c:axId val="-2058765056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -914,7 +914,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102009920"/>
+        <c:crossAx val="-2132201952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -922,7 +922,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2102009920"/>
+        <c:axId val="-2132201952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -989,7 +989,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102006640"/>
+        <c:crossAx val="-2058765056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1589,11 +1589,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="-2098751824"/>
-        <c:axId val="-2098748640"/>
+        <c:axId val="-2136968784"/>
+        <c:axId val="-2136965216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2098751824"/>
+        <c:axId val="-2136968784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,7 +1650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098748640"/>
+        <c:crossAx val="-2136965216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1658,7 +1658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2098748640"/>
+        <c:axId val="-2136965216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1725,7 +1725,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098751824"/>
+        <c:crossAx val="-2136968784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1957,11 +1957,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2099512224"/>
-        <c:axId val="-2099507040"/>
+        <c:axId val="-2058751920"/>
+        <c:axId val="-2058746640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2099512224"/>
+        <c:axId val="-2058751920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,7 +1990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099507040"/>
+        <c:crossAx val="-2058746640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1998,7 +1998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2099507040"/>
+        <c:axId val="-2058746640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2037,7 +2037,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099512224"/>
+        <c:crossAx val="-2058751920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2061,10 +2061,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -2076,6 +2076,96 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$53:$A$58</c:f>
@@ -2141,16 +2231,75 @@
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -2303,11 +2452,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2099442384"/>
-        <c:axId val="-2099439456"/>
+        <c:axId val="-2058681872"/>
+        <c:axId val="-2058678944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2099442384"/>
+        <c:axId val="-2058681872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2317,7 +2466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099439456"/>
+        <c:crossAx val="-2058678944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2325,7 +2474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2099439456"/>
+        <c:axId val="-2058678944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2336,7 +2485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099442384"/>
+        <c:crossAx val="-2058681872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2438,6 +2587,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
   <cs:axisTitle>
@@ -3482,6 +3671,525 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3965,8 +4673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>